<commit_message>
bug fix for building upgrade
</commit_message>
<xml_diff>
--- a/gameData/shared/GemsPayment.xlsx
+++ b/gameData/shared/GemsPayment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="3900" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="6"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="time" sheetId="2" r:id="rId1"/>
@@ -73,14 +73,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>FLOAT_speedup</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>FLOAT_resource</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>INT_tools</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -110,6 +102,14 @@
   </si>
   <si>
     <t>INT_ironPart</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_speedup</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_resource</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -259,7 +259,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="70">
+  <cellStyleXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -334,6 +334,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -347,7 +349,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="70">
+  <cellStyles count="72">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -385,6 +387,7 @@
     <cellStyle name="超链接" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="70" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -415,6 +418,7 @@
     <cellStyle name="访问过的超链接" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="71" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -867,7 +871,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -886,7 +890,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1042,7 +1046,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1061,7 +1065,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1166,7 +1170,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1185,7 +1189,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1290,7 +1294,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1309,7 +1313,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1414,7 +1418,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1433,7 +1437,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1538,7 +1542,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1557,7 +1561,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1675,28 +1679,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="20" customHeight="1">

</xml_diff>

<commit_message>
fix dev of feathur_house
</commit_message>
<xml_diff>
--- a/gameData/shared/GemsPayment.xlsx
+++ b/gameData/shared/GemsPayment.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="6"/>
+    <workbookView xWindow="1640" yWindow="0" windowWidth="31940" windowHeight="18740" tabRatio="883" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="time" sheetId="2" r:id="rId1"/>
@@ -13,34 +13,39 @@
     <sheet name="iron" sheetId="6" r:id="rId4"/>
     <sheet name="food" sheetId="7" r:id="rId5"/>
     <sheet name="coin" sheetId="8" r:id="rId6"/>
-    <sheet name="material" sheetId="10" r:id="rId7"/>
+    <sheet name="citizen" sheetId="12" r:id="rId7"/>
+    <sheet name="material" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="6">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="5">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="3">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="7">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="6">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="5">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="3">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="7">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="6">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="5">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="3">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="7">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="6">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="5">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="4">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="3">#REF!</definedName>
-    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="7">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8">#REF!</definedName>
@@ -55,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
   <si>
     <t>INT_index</t>
     <phoneticPr fontId="10" type="noConversion"/>
@@ -1046,7 +1051,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1663,9 +1668,133 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="20.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="20" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20" customHeight="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="D2" s="1">
+        <v>300</v>
+      </c>
+      <c r="E2" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1201</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3750</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1500</v>
+      </c>
+      <c r="E3" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20" customHeight="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3751</v>
+      </c>
+      <c r="C4" s="1">
+        <v>15000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>15001</v>
+      </c>
+      <c r="C5" s="1">
+        <v>55000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>20000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" customHeight="1">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>55001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>60000</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3300</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bugfix for gem not a number
</commit_message>
<xml_diff>
--- a/gameData/shared/GemsPayment.xlsx
+++ b/gameData/shared/GemsPayment.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="0" windowWidth="31940" windowHeight="18740" tabRatio="883" activeTab="6"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="883" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="time" sheetId="2" r:id="rId1"/>
@@ -94,19 +94,7 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>INT_bowTarget</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>INT_saddle</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_bluePrints</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_ironPart</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -115,6 +103,18 @@
   </si>
   <si>
     <t>INT_resource</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_blueprints</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_bowTarget</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_ironPart</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -895,7 +895,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1070,7 +1070,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1194,7 +1194,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1318,7 +1318,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1442,7 +1442,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1566,7 +1566,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1670,7 +1670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1690,7 +1690,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1794,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1808,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>4</v>
@@ -1823,13 +1823,13 @@
         <v>7</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="20" customHeight="1">

</xml_diff>

<commit_message>
finish dev of barracks
</commit_message>
<xml_diff>
--- a/gameData/shared/GemsPayment.xlsx
+++ b/gameData/shared/GemsPayment.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="883" activeTab="7"/>
+    <workbookView xWindow="6960" yWindow="3260" windowWidth="25040" windowHeight="15500" tabRatio="883" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="time" sheetId="2" r:id="rId1"/>
@@ -1794,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>